<commit_message>
stcode11 changed to code11
</commit_message>
<xml_diff>
--- a/data-raw/state_abbr.xlsx
+++ b/data-raw/state_abbr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umassmed-my.sharepoint.com/personal/shubham_dutta_umassmed_edu/Documents/01_Personal/00_Important_main/02_R-projects/00_Packages/93_indiamap/indiamapdata/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{005E45BA-ACC0-9C46-B15A-D78A7456844E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8A430B3-1A79-1746-B152-4A28559E338B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{005E45BA-ACC0-9C46-B15A-D78A7456844E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA490449-EC62-5E4D-8281-4F90E6AF1C73}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3E90E0BD-16F1-5644-9975-D49FAD586033}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>abbr</t>
   </si>
   <si>
-    <t>stcode11</t>
-  </si>
-  <si>
     <t>AN</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>05</t>
+  </si>
+  <si>
+    <t>code11</t>
   </si>
 </sst>
 </file>
@@ -706,6 +706,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,7 +1032,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,12 +1045,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>35</v>
@@ -1054,7 +1058,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>37</v>
@@ -1062,7 +1066,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1070,7 +1074,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>18</v>
@@ -1078,7 +1082,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>10</v>
@@ -1086,15 +1090,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>22</v>
@@ -1102,7 +1106,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>26</v>
@@ -1110,7 +1114,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>25</v>
@@ -1118,15 +1122,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>30</v>
@@ -1134,7 +1138,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>24</v>
@@ -1142,31 +1146,31 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>20</v>
@@ -1174,7 +1178,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>29</v>
@@ -1182,7 +1186,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>32</v>
@@ -1190,7 +1194,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>38</v>
@@ -1198,7 +1202,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>31</v>
@@ -1206,7 +1210,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>23</v>
@@ -1214,7 +1218,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>27</v>
@@ -1222,7 +1226,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>14</v>
@@ -1230,7 +1234,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>17</v>
@@ -1238,7 +1242,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>15</v>
@@ -1246,7 +1250,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>13</v>
@@ -1254,7 +1258,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>21</v>
@@ -1262,7 +1266,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>34</v>
@@ -1270,23 +1274,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>11</v>
@@ -1294,7 +1298,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>33</v>
@@ -1302,7 +1306,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>36</v>
@@ -1310,7 +1314,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>16</v>
@@ -1318,23 +1322,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>19</v>

</xml_diff>